<commit_message>
check in advance poll stuff
</commit_message>
<xml_diff>
--- a/campaign/Advance Poll Kit/AdvancePoll.xlsx
+++ b/campaign/Advance Poll Kit/AdvancePoll.xlsx
@@ -5237,7 +5237,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:R407"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
@@ -5252,7 +5251,7 @@
     <col min="12" max="12" width="19.85546875" customWidth="1"/>
     <col min="13" max="13" width="16.5703125" customWidth="1"/>
     <col min="14" max="14" width="16.5703125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -5361,7 +5360,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:18" hidden="1">
+    <row r="3" spans="1:18">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
@@ -5413,7 +5412,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:18" hidden="1">
+    <row r="4" spans="1:18">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
@@ -5465,7 +5464,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:18" hidden="1">
+    <row r="5" spans="1:18">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -5517,7 +5516,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:18" hidden="1">
+    <row r="6" spans="1:18">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
@@ -5569,7 +5568,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:18" hidden="1">
+    <row r="7" spans="1:18">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
@@ -5673,7 +5672,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:18" hidden="1">
+    <row r="9" spans="1:18">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
@@ -5723,7 +5722,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:18" hidden="1">
+    <row r="10" spans="1:18">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
@@ -5773,7 +5772,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:18" hidden="1">
+    <row r="11" spans="1:18">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
@@ -5823,7 +5822,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:18" hidden="1">
+    <row r="12" spans="1:18">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
@@ -5875,7 +5874,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:18" hidden="1">
+    <row r="13" spans="1:18">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
@@ -5927,7 +5926,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:18" hidden="1">
+    <row r="14" spans="1:18">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
@@ -5979,7 +5978,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:18" hidden="1">
+    <row r="15" spans="1:18">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
@@ -6239,7 +6238,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:18" hidden="1">
+    <row r="20" spans="1:18">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
@@ -6291,7 +6290,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:18" hidden="1">
+    <row r="21" spans="1:18">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
@@ -6343,7 +6342,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:18" hidden="1">
+    <row r="22" spans="1:18">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
@@ -6395,7 +6394,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:18" hidden="1">
+    <row r="23" spans="1:18">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
@@ -6447,7 +6446,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:18" hidden="1">
+    <row r="24" spans="1:18">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
@@ -6811,7 +6810,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:18" hidden="1">
+    <row r="31" spans="1:18">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
@@ -6863,7 +6862,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:18" hidden="1">
+    <row r="32" spans="1:18">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
@@ -6915,7 +6914,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:18" hidden="1">
+    <row r="33" spans="1:18">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
@@ -6967,7 +6966,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:18" hidden="1">
+    <row r="34" spans="1:18">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
@@ -7019,7 +7018,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:18" hidden="1">
+    <row r="35" spans="1:18">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
@@ -7071,7 +7070,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="1:18" hidden="1">
+    <row r="36" spans="1:18">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
@@ -7279,7 +7278,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:18" hidden="1">
+    <row r="40" spans="1:18">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
@@ -7331,7 +7330,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="41" spans="1:18" hidden="1">
+    <row r="41" spans="1:18">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
@@ -8215,7 +8214,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="1:18" hidden="1">
+    <row r="58" spans="1:18">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
@@ -8267,7 +8266,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="59" spans="1:18" hidden="1">
+    <row r="59" spans="1:18">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
@@ -8683,7 +8682,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="1:18" hidden="1">
+    <row r="67" spans="1:18">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2" t="s">
@@ -8733,7 +8732,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="68" spans="1:18" hidden="1">
+    <row r="68" spans="1:18">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2" t="s">
@@ -8783,7 +8782,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="69" spans="1:18" hidden="1">
+    <row r="69" spans="1:18">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2" t="s">
@@ -8833,7 +8832,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="70" spans="1:18" hidden="1">
+    <row r="70" spans="1:18">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2" t="s">
@@ -8885,7 +8884,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="71" spans="1:18" hidden="1">
+    <row r="71" spans="1:18">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2" t="s">
@@ -8937,7 +8936,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="72" spans="1:18" hidden="1">
+    <row r="72" spans="1:18">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
@@ -8989,7 +8988,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="73" spans="1:18" hidden="1">
+    <row r="73" spans="1:18">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2" t="s">
@@ -9299,7 +9298,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="79" spans="1:18" hidden="1">
+    <row r="79" spans="1:18">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2" t="s">
@@ -9349,7 +9348,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="80" spans="1:18" hidden="1">
+    <row r="80" spans="1:18">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2" t="s">
@@ -9399,7 +9398,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="81" spans="1:18" hidden="1">
+    <row r="81" spans="1:18">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2" t="s">
@@ -9449,7 +9448,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="82" spans="1:18" hidden="1">
+    <row r="82" spans="1:18">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2" t="s">
@@ -9499,7 +9498,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="83" spans="1:18" hidden="1">
+    <row r="83" spans="1:18">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2" t="s">
@@ -9549,7 +9548,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="84" spans="1:18" hidden="1">
+    <row r="84" spans="1:18">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2" t="s">
@@ -9599,7 +9598,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="85" spans="1:18" hidden="1">
+    <row r="85" spans="1:18">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2" t="s">
@@ -9649,7 +9648,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="86" spans="1:18" hidden="1">
+    <row r="86" spans="1:18">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2" t="s">
@@ -9857,7 +9856,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="90" spans="1:18" hidden="1">
+    <row r="90" spans="1:18">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2" t="s">
@@ -9907,7 +9906,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="91" spans="1:18" hidden="1">
+    <row r="91" spans="1:18">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2" t="s">
@@ -9957,7 +9956,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="92" spans="1:18" hidden="1">
+    <row r="92" spans="1:18">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2" t="s">
@@ -10007,7 +10006,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="93" spans="1:18" hidden="1">
+    <row r="93" spans="1:18">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2" t="s">
@@ -10059,7 +10058,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="94" spans="1:18" hidden="1">
+    <row r="94" spans="1:18">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2" t="s">
@@ -10111,7 +10110,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="95" spans="1:18" hidden="1">
+    <row r="95" spans="1:18">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2" t="s">
@@ -10163,7 +10162,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="96" spans="1:18" hidden="1">
+    <row r="96" spans="1:18">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2" t="s">
@@ -10213,7 +10212,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="97" spans="1:18" hidden="1">
+    <row r="97" spans="1:18">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2" t="s">
@@ -10265,7 +10264,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="98" spans="1:18" hidden="1">
+    <row r="98" spans="1:18">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2" t="s">
@@ -10315,7 +10314,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="99" spans="1:18" hidden="1">
+    <row r="99" spans="1:18">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2" t="s">
@@ -10365,7 +10364,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="100" spans="1:18" hidden="1">
+    <row r="100" spans="1:18">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2" t="s">
@@ -10415,7 +10414,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="101" spans="1:18" hidden="1">
+    <row r="101" spans="1:18">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2" t="s">
@@ -10467,7 +10466,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="102" spans="1:18" hidden="1">
+    <row r="102" spans="1:18">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2" t="s">
@@ -10519,7 +10518,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="103" spans="1:18" hidden="1">
+    <row r="103" spans="1:18">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2" t="s">
@@ -10569,7 +10568,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="104" spans="1:18" hidden="1">
+    <row r="104" spans="1:18">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2" t="s">
@@ -10621,7 +10620,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="105" spans="1:18" hidden="1">
+    <row r="105" spans="1:18">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2" t="s">
@@ -10673,7 +10672,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="106" spans="1:18" hidden="1">
+    <row r="106" spans="1:18">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2" t="s">
@@ -10725,7 +10724,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="107" spans="1:18" hidden="1">
+    <row r="107" spans="1:18">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2" t="s">
@@ -10777,7 +10776,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="108" spans="1:18" hidden="1">
+    <row r="108" spans="1:18">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2" t="s">
@@ -10933,7 +10932,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="111" spans="1:18" hidden="1">
+    <row r="111" spans="1:18">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2" t="s">
@@ -10985,7 +10984,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="112" spans="1:18" hidden="1">
+    <row r="112" spans="1:18">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2" t="s">
@@ -11037,7 +11036,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="113" spans="1:18" hidden="1">
+    <row r="113" spans="1:18">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2" t="s">
@@ -11193,7 +11192,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="116" spans="1:18" hidden="1">
+    <row r="116" spans="1:18">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2" t="s">
@@ -11245,7 +11244,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="117" spans="1:18" hidden="1">
+    <row r="117" spans="1:18">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2" t="s">
@@ -11297,7 +11296,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="118" spans="1:18" hidden="1">
+    <row r="118" spans="1:18">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2" t="s">
@@ -11349,7 +11348,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="119" spans="1:18" hidden="1">
+    <row r="119" spans="1:18">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2" t="s">
@@ -11505,7 +11504,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="122" spans="1:18" hidden="1">
+    <row r="122" spans="1:18">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2" t="s">
@@ -11555,7 +11554,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="123" spans="1:18" hidden="1">
+    <row r="123" spans="1:18">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2" t="s">
@@ -11607,7 +11606,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="124" spans="1:18" hidden="1">
+    <row r="124" spans="1:18">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2" t="s">
@@ -11659,7 +11658,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="125" spans="1:18" hidden="1">
+    <row r="125" spans="1:18">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2" t="s">
@@ -11711,7 +11710,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="126" spans="1:18" hidden="1">
+    <row r="126" spans="1:18">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2" t="s">
@@ -12335,7 +12334,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="138" spans="1:18" hidden="1">
+    <row r="138" spans="1:18">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2" t="s">
@@ -12387,7 +12386,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="139" spans="1:18" hidden="1">
+    <row r="139" spans="1:18">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2" t="s">
@@ -12439,7 +12438,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="140" spans="1:18" hidden="1">
+    <row r="140" spans="1:18">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2" t="s">
@@ -12491,7 +12490,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="141" spans="1:18" hidden="1">
+    <row r="141" spans="1:18">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2" t="s">
@@ -12595,7 +12594,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="143" spans="1:18" hidden="1">
+    <row r="143" spans="1:18">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2" t="s">
@@ -12647,7 +12646,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="144" spans="1:18" hidden="1">
+    <row r="144" spans="1:18">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2" t="s">
@@ -12699,7 +12698,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="145" spans="1:18" hidden="1">
+    <row r="145" spans="1:18">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2" t="s">
@@ -12751,7 +12750,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="146" spans="1:18" hidden="1">
+    <row r="146" spans="1:18">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2" t="s">
@@ -12803,7 +12802,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="147" spans="1:18" hidden="1">
+    <row r="147" spans="1:18">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2" t="s">
@@ -12855,7 +12854,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="148" spans="1:18" hidden="1">
+    <row r="148" spans="1:18">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2" t="s">
@@ -12907,7 +12906,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="149" spans="1:18" hidden="1">
+    <row r="149" spans="1:18">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2" t="s">
@@ -12959,7 +12958,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="150" spans="1:18" hidden="1">
+    <row r="150" spans="1:18">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2" t="s">
@@ -13011,7 +13010,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="151" spans="1:18" hidden="1">
+    <row r="151" spans="1:18">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2" t="s">
@@ -13063,7 +13062,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="152" spans="1:18" hidden="1">
+    <row r="152" spans="1:18">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2" t="s">
@@ -13167,7 +13166,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="154" spans="1:18" hidden="1">
+    <row r="154" spans="1:18">
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2" t="s">
@@ -13219,7 +13218,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="155" spans="1:18" hidden="1">
+    <row r="155" spans="1:18">
       <c r="A155" s="2"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2" t="s">
@@ -13271,7 +13270,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="156" spans="1:18" hidden="1">
+    <row r="156" spans="1:18">
       <c r="A156" s="2"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2" t="s">
@@ -13323,7 +13322,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="157" spans="1:18" hidden="1">
+    <row r="157" spans="1:18">
       <c r="A157" s="2"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2" t="s">
@@ -13375,7 +13374,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="158" spans="1:18" hidden="1">
+    <row r="158" spans="1:18">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2" t="s">
@@ -13427,7 +13426,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="159" spans="1:18" hidden="1">
+    <row r="159" spans="1:18">
       <c r="A159" s="2"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2" t="s">
@@ -13479,7 +13478,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="160" spans="1:18" hidden="1">
+    <row r="160" spans="1:18">
       <c r="A160" s="2"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2" t="s">
@@ -13531,7 +13530,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="161" spans="1:18" hidden="1">
+    <row r="161" spans="1:18">
       <c r="A161" s="2"/>
       <c r="B161" s="2"/>
       <c r="C161" s="2" t="s">
@@ -13583,7 +13582,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="162" spans="1:18" hidden="1">
+    <row r="162" spans="1:18">
       <c r="A162" s="2"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2" t="s">
@@ -13635,7 +13634,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="163" spans="1:18" hidden="1">
+    <row r="163" spans="1:18">
       <c r="A163" s="2"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2" t="s">
@@ -13687,7 +13686,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="164" spans="1:18" hidden="1">
+    <row r="164" spans="1:18">
       <c r="A164" s="2"/>
       <c r="B164" s="2"/>
       <c r="C164" s="2" t="s">
@@ -14099,7 +14098,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="172" spans="1:18" hidden="1">
+    <row r="172" spans="1:18">
       <c r="A172" s="2"/>
       <c r="B172" s="2"/>
       <c r="C172" s="2" t="s">
@@ -14151,7 +14150,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="173" spans="1:18" hidden="1">
+    <row r="173" spans="1:18">
       <c r="A173" s="2"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2" t="s">
@@ -14203,7 +14202,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="174" spans="1:18" hidden="1">
+    <row r="174" spans="1:18">
       <c r="A174" s="2"/>
       <c r="B174" s="2"/>
       <c r="C174" s="2" t="s">
@@ -14255,7 +14254,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="175" spans="1:18" hidden="1">
+    <row r="175" spans="1:18">
       <c r="A175" s="2"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2" t="s">
@@ -14305,7 +14304,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="176" spans="1:18" hidden="1">
+    <row r="176" spans="1:18">
       <c r="A176" s="2"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2" t="s">
@@ -14355,7 +14354,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="177" spans="1:18" hidden="1">
+    <row r="177" spans="1:18">
       <c r="A177" s="2"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2" t="s">
@@ -14405,7 +14404,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="178" spans="1:18" hidden="1">
+    <row r="178" spans="1:18">
       <c r="A178" s="2"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2" t="s">
@@ -14455,7 +14454,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="179" spans="1:18" hidden="1">
+    <row r="179" spans="1:18">
       <c r="A179" s="2"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2" t="s">
@@ -14505,7 +14504,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="180" spans="1:18" hidden="1">
+    <row r="180" spans="1:18">
       <c r="A180" s="2"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2" t="s">
@@ -14555,7 +14554,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="181" spans="1:18" hidden="1">
+    <row r="181" spans="1:18">
       <c r="A181" s="2"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2" t="s">
@@ -14605,7 +14604,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="182" spans="1:18" hidden="1">
+    <row r="182" spans="1:18">
       <c r="A182" s="2"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2" t="s">
@@ -14655,7 +14654,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="183" spans="1:18" hidden="1">
+    <row r="183" spans="1:18">
       <c r="A183" s="2"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2" t="s">
@@ -14705,7 +14704,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="184" spans="1:18" hidden="1">
+    <row r="184" spans="1:18">
       <c r="A184" s="2"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2" t="s">
@@ -14755,7 +14754,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="185" spans="1:18" hidden="1">
+    <row r="185" spans="1:18">
       <c r="A185" s="2"/>
       <c r="B185" s="2"/>
       <c r="C185" s="2" t="s">
@@ -14805,7 +14804,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="186" spans="1:18" hidden="1">
+    <row r="186" spans="1:18">
       <c r="A186" s="2"/>
       <c r="B186" s="2"/>
       <c r="C186" s="2" t="s">
@@ -14855,7 +14854,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="187" spans="1:18" hidden="1">
+    <row r="187" spans="1:18">
       <c r="A187" s="2"/>
       <c r="B187" s="2"/>
       <c r="C187" s="2" t="s">
@@ -14905,7 +14904,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="188" spans="1:18" hidden="1">
+    <row r="188" spans="1:18">
       <c r="A188" s="2"/>
       <c r="B188" s="2"/>
       <c r="C188" s="2" t="s">
@@ -14955,7 +14954,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="189" spans="1:18" hidden="1">
+    <row r="189" spans="1:18">
       <c r="A189" s="2"/>
       <c r="B189" s="2"/>
       <c r="C189" s="2" t="s">
@@ -15005,7 +15004,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="190" spans="1:18" hidden="1">
+    <row r="190" spans="1:18">
       <c r="A190" s="2"/>
       <c r="B190" s="2"/>
       <c r="C190" s="2" t="s">
@@ -15263,7 +15262,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="195" spans="1:18" hidden="1">
+    <row r="195" spans="1:18">
       <c r="A195" s="2"/>
       <c r="B195" s="2"/>
       <c r="C195" s="2" t="s">
@@ -15315,7 +15314,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="196" spans="1:18" hidden="1">
+    <row r="196" spans="1:18">
       <c r="A196" s="2"/>
       <c r="B196" s="2"/>
       <c r="C196" s="2" t="s">
@@ -15367,7 +15366,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="197" spans="1:18" hidden="1">
+    <row r="197" spans="1:18">
       <c r="A197" s="2"/>
       <c r="B197" s="2"/>
       <c r="C197" s="2" t="s">
@@ -15419,7 +15418,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="198" spans="1:18" hidden="1">
+    <row r="198" spans="1:18">
       <c r="A198" s="2"/>
       <c r="B198" s="2"/>
       <c r="C198" s="2" t="s">
@@ -15469,7 +15468,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="199" spans="1:18" hidden="1">
+    <row r="199" spans="1:18">
       <c r="A199" s="2"/>
       <c r="B199" s="2"/>
       <c r="C199" s="2" t="s">
@@ -15519,7 +15518,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="200" spans="1:18" hidden="1">
+    <row r="200" spans="1:18">
       <c r="A200" s="2"/>
       <c r="B200" s="2"/>
       <c r="C200" s="2" t="s">
@@ -15569,7 +15568,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="201" spans="1:18" hidden="1">
+    <row r="201" spans="1:18">
       <c r="A201" s="2"/>
       <c r="B201" s="2"/>
       <c r="C201" s="2" t="s">
@@ -15619,7 +15618,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="202" spans="1:18" hidden="1">
+    <row r="202" spans="1:18">
       <c r="A202" s="2"/>
       <c r="B202" s="2"/>
       <c r="C202" s="2" t="s">
@@ -15929,7 +15928,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="208" spans="1:18" hidden="1">
+    <row r="208" spans="1:18">
       <c r="A208" s="2"/>
       <c r="B208" s="2"/>
       <c r="C208" s="2" t="s">
@@ -15981,7 +15980,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="209" spans="1:18" hidden="1">
+    <row r="209" spans="1:18">
       <c r="A209" s="2"/>
       <c r="B209" s="2"/>
       <c r="C209" s="2" t="s">
@@ -16033,7 +16032,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="210" spans="1:18" hidden="1">
+    <row r="210" spans="1:18">
       <c r="A210" s="2"/>
       <c r="B210" s="2"/>
       <c r="C210" s="2" t="s">
@@ -16085,7 +16084,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="211" spans="1:18" hidden="1">
+    <row r="211" spans="1:18">
       <c r="A211" s="2"/>
       <c r="B211" s="2"/>
       <c r="C211" s="2" t="s">
@@ -16137,7 +16136,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="212" spans="1:18" hidden="1">
+    <row r="212" spans="1:18">
       <c r="A212" s="2"/>
       <c r="B212" s="2"/>
       <c r="C212" s="2" t="s">
@@ -16189,7 +16188,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="213" spans="1:18" hidden="1">
+    <row r="213" spans="1:18">
       <c r="A213" s="2"/>
       <c r="B213" s="2"/>
       <c r="C213" s="2" t="s">
@@ -16241,7 +16240,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="214" spans="1:18" hidden="1">
+    <row r="214" spans="1:18">
       <c r="A214" s="2"/>
       <c r="B214" s="2"/>
       <c r="C214" s="2" t="s">
@@ -16293,7 +16292,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="215" spans="1:18" hidden="1">
+    <row r="215" spans="1:18">
       <c r="A215" s="2"/>
       <c r="B215" s="2"/>
       <c r="C215" s="2" t="s">
@@ -16345,7 +16344,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="216" spans="1:18" hidden="1">
+    <row r="216" spans="1:18">
       <c r="A216" s="2"/>
       <c r="B216" s="2"/>
       <c r="C216" s="2" t="s">
@@ -16397,7 +16396,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="217" spans="1:18" hidden="1">
+    <row r="217" spans="1:18">
       <c r="A217" s="2"/>
       <c r="B217" s="2"/>
       <c r="C217" s="2" t="s">
@@ -16449,7 +16448,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="218" spans="1:18" hidden="1">
+    <row r="218" spans="1:18">
       <c r="A218" s="2"/>
       <c r="B218" s="2"/>
       <c r="C218" s="2" t="s">
@@ -16501,7 +16500,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="219" spans="1:18" hidden="1">
+    <row r="219" spans="1:18">
       <c r="A219" s="2"/>
       <c r="B219" s="2"/>
       <c r="C219" s="2" t="s">
@@ -16553,7 +16552,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="220" spans="1:18" hidden="1">
+    <row r="220" spans="1:18">
       <c r="A220" s="2"/>
       <c r="B220" s="2"/>
       <c r="C220" s="2" t="s">
@@ -16605,7 +16604,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="221" spans="1:18" hidden="1">
+    <row r="221" spans="1:18">
       <c r="A221" s="2"/>
       <c r="B221" s="2"/>
       <c r="C221" s="2" t="s">
@@ -16655,7 +16654,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="222" spans="1:18" hidden="1">
+    <row r="222" spans="1:18">
       <c r="A222" s="2"/>
       <c r="B222" s="2"/>
       <c r="C222" s="2" t="s">
@@ -16705,7 +16704,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="223" spans="1:18" hidden="1">
+    <row r="223" spans="1:18">
       <c r="A223" s="2"/>
       <c r="B223" s="2"/>
       <c r="C223" s="2" t="s">
@@ -16755,7 +16754,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="224" spans="1:18" hidden="1">
+    <row r="224" spans="1:18">
       <c r="A224" s="2"/>
       <c r="B224" s="2"/>
       <c r="C224" s="2" t="s">
@@ -16805,7 +16804,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="225" spans="1:18" hidden="1">
+    <row r="225" spans="1:18">
       <c r="A225" s="2"/>
       <c r="B225" s="2"/>
       <c r="C225" s="2" t="s">
@@ -16855,7 +16854,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="226" spans="1:18" hidden="1">
+    <row r="226" spans="1:18">
       <c r="A226" s="2"/>
       <c r="B226" s="2"/>
       <c r="C226" s="2" t="s">
@@ -16905,7 +16904,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="227" spans="1:18" hidden="1">
+    <row r="227" spans="1:18">
       <c r="A227" s="2"/>
       <c r="B227" s="2"/>
       <c r="C227" s="2" t="s">
@@ -16957,7 +16956,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="228" spans="1:18" hidden="1">
+    <row r="228" spans="1:18">
       <c r="A228" s="2"/>
       <c r="B228" s="2"/>
       <c r="C228" s="2" t="s">
@@ -17269,7 +17268,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="234" spans="1:18" hidden="1">
+    <row r="234" spans="1:18">
       <c r="A234" s="2"/>
       <c r="B234" s="2"/>
       <c r="C234" s="2" t="s">
@@ -17321,7 +17320,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="235" spans="1:18" hidden="1">
+    <row r="235" spans="1:18">
       <c r="A235" s="2"/>
       <c r="B235" s="2"/>
       <c r="C235" s="2" t="s">
@@ -17373,7 +17372,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="236" spans="1:18" hidden="1">
+    <row r="236" spans="1:18">
       <c r="A236" s="2"/>
       <c r="B236" s="2"/>
       <c r="C236" s="2" t="s">
@@ -17631,7 +17630,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="241" spans="1:18" hidden="1">
+    <row r="241" spans="1:18">
       <c r="A241" s="2"/>
       <c r="B241" s="2"/>
       <c r="C241" s="2" t="s">
@@ -17683,7 +17682,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="242" spans="1:18" hidden="1">
+    <row r="242" spans="1:18">
       <c r="A242" s="2"/>
       <c r="B242" s="2"/>
       <c r="C242" s="2" t="s">
@@ -17735,7 +17734,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="243" spans="1:18" hidden="1">
+    <row r="243" spans="1:18">
       <c r="A243" s="2"/>
       <c r="B243" s="2"/>
       <c r="C243" s="2" t="s">
@@ -17787,7 +17786,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="244" spans="1:18" hidden="1">
+    <row r="244" spans="1:18">
       <c r="A244" s="2"/>
       <c r="B244" s="2"/>
       <c r="C244" s="2" t="s">
@@ -17839,7 +17838,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="245" spans="1:18" hidden="1">
+    <row r="245" spans="1:18">
       <c r="A245" s="2"/>
       <c r="B245" s="2"/>
       <c r="C245" s="2" t="s">
@@ -17891,7 +17890,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="246" spans="1:18" hidden="1">
+    <row r="246" spans="1:18">
       <c r="A246" s="2"/>
       <c r="B246" s="2"/>
       <c r="C246" s="2" t="s">
@@ -17943,7 +17942,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="247" spans="1:18" hidden="1">
+    <row r="247" spans="1:18">
       <c r="A247" s="2"/>
       <c r="B247" s="2"/>
       <c r="C247" s="2" t="s">
@@ -17995,7 +17994,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="248" spans="1:18" hidden="1">
+    <row r="248" spans="1:18">
       <c r="A248" s="2"/>
       <c r="B248" s="2"/>
       <c r="C248" s="2" t="s">
@@ -18047,7 +18046,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="249" spans="1:18" hidden="1">
+    <row r="249" spans="1:18">
       <c r="A249" s="2"/>
       <c r="B249" s="2"/>
       <c r="C249" s="2" t="s">
@@ -18099,7 +18098,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="250" spans="1:18" hidden="1">
+    <row r="250" spans="1:18">
       <c r="A250" s="2"/>
       <c r="B250" s="2"/>
       <c r="C250" s="2" t="s">
@@ -18151,7 +18150,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="251" spans="1:18" hidden="1">
+    <row r="251" spans="1:18">
       <c r="A251" s="2"/>
       <c r="B251" s="2"/>
       <c r="C251" s="2" t="s">
@@ -18201,7 +18200,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="252" spans="1:18" hidden="1">
+    <row r="252" spans="1:18">
       <c r="A252" s="2"/>
       <c r="B252" s="2"/>
       <c r="C252" s="2" t="s">
@@ -18251,7 +18250,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="253" spans="1:18" hidden="1">
+    <row r="253" spans="1:18">
       <c r="A253" s="2"/>
       <c r="B253" s="2"/>
       <c r="C253" s="2" t="s">
@@ -18301,7 +18300,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="254" spans="1:18" hidden="1">
+    <row r="254" spans="1:18">
       <c r="A254" s="2"/>
       <c r="B254" s="2"/>
       <c r="C254" s="2" t="s">
@@ -18351,7 +18350,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="255" spans="1:18" hidden="1">
+    <row r="255" spans="1:18">
       <c r="A255" s="2"/>
       <c r="B255" s="2"/>
       <c r="C255" s="2" t="s">
@@ -18401,7 +18400,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="256" spans="1:18" hidden="1">
+    <row r="256" spans="1:18">
       <c r="A256" s="2"/>
       <c r="B256" s="2"/>
       <c r="C256" s="2" t="s">
@@ -18451,7 +18450,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="257" spans="1:18" hidden="1">
+    <row r="257" spans="1:18">
       <c r="A257" s="2"/>
       <c r="B257" s="2"/>
       <c r="C257" s="2" t="s">
@@ -18501,7 +18500,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="258" spans="1:18" hidden="1">
+    <row r="258" spans="1:18">
       <c r="A258" s="2"/>
       <c r="B258" s="2"/>
       <c r="C258" s="2" t="s">
@@ -18551,7 +18550,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="259" spans="1:18" hidden="1">
+    <row r="259" spans="1:18">
       <c r="A259" s="2"/>
       <c r="B259" s="2"/>
       <c r="C259" s="2" t="s">
@@ -18601,7 +18600,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="260" spans="1:18" hidden="1">
+    <row r="260" spans="1:18">
       <c r="A260" s="2"/>
       <c r="B260" s="2"/>
       <c r="C260" s="2" t="s">
@@ -18651,7 +18650,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="261" spans="1:18" hidden="1">
+    <row r="261" spans="1:18">
       <c r="A261" s="2"/>
       <c r="B261" s="2"/>
       <c r="C261" s="2" t="s">
@@ -18701,7 +18700,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="262" spans="1:18" hidden="1">
+    <row r="262" spans="1:18">
       <c r="A262" s="2"/>
       <c r="B262" s="2"/>
       <c r="C262" s="2" t="s">
@@ -18751,7 +18750,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="263" spans="1:18" hidden="1">
+    <row r="263" spans="1:18">
       <c r="A263" s="2"/>
       <c r="B263" s="2"/>
       <c r="C263" s="2" t="s">
@@ -18801,7 +18800,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="264" spans="1:18" hidden="1">
+    <row r="264" spans="1:18">
       <c r="A264" s="2"/>
       <c r="B264" s="2"/>
       <c r="C264" s="2" t="s">
@@ -18851,7 +18850,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="265" spans="1:18" hidden="1">
+    <row r="265" spans="1:18">
       <c r="A265" s="2"/>
       <c r="B265" s="2"/>
       <c r="C265" s="2" t="s">
@@ -18901,7 +18900,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="266" spans="1:18" hidden="1">
+    <row r="266" spans="1:18">
       <c r="A266" s="2"/>
       <c r="B266" s="2"/>
       <c r="C266" s="2" t="s">
@@ -18951,7 +18950,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="267" spans="1:18" hidden="1">
+    <row r="267" spans="1:18">
       <c r="A267" s="2"/>
       <c r="B267" s="2"/>
       <c r="C267" s="2" t="s">
@@ -19001,7 +19000,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="268" spans="1:18" hidden="1">
+    <row r="268" spans="1:18">
       <c r="A268" s="2"/>
       <c r="B268" s="2"/>
       <c r="C268" s="2" t="s">
@@ -19051,7 +19050,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="269" spans="1:18" hidden="1">
+    <row r="269" spans="1:18">
       <c r="A269" s="2"/>
       <c r="B269" s="2"/>
       <c r="C269" s="2" t="s">
@@ -19101,7 +19100,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="270" spans="1:18" hidden="1">
+    <row r="270" spans="1:18">
       <c r="A270" s="2"/>
       <c r="B270" s="2"/>
       <c r="C270" s="2" t="s">
@@ -19151,7 +19150,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="271" spans="1:18" hidden="1">
+    <row r="271" spans="1:18">
       <c r="A271" s="2"/>
       <c r="B271" s="2"/>
       <c r="C271" s="2" t="s">
@@ -19201,7 +19200,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="272" spans="1:18" hidden="1">
+    <row r="272" spans="1:18">
       <c r="A272" s="2"/>
       <c r="B272" s="2"/>
       <c r="C272" s="2" t="s">
@@ -19251,7 +19250,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="273" spans="1:18" hidden="1">
+    <row r="273" spans="1:18">
       <c r="A273" s="2"/>
       <c r="B273" s="2"/>
       <c r="C273" s="2" t="s">
@@ -19301,7 +19300,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="274" spans="1:18" hidden="1">
+    <row r="274" spans="1:18">
       <c r="A274" s="2"/>
       <c r="B274" s="2"/>
       <c r="C274" s="2" t="s">
@@ -19351,7 +19350,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="275" spans="1:18" hidden="1">
+    <row r="275" spans="1:18">
       <c r="A275" s="2"/>
       <c r="B275" s="2"/>
       <c r="C275" s="2" t="s">
@@ -19401,7 +19400,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="276" spans="1:18" hidden="1">
+    <row r="276" spans="1:18">
       <c r="A276" s="2"/>
       <c r="B276" s="2"/>
       <c r="C276" s="2" t="s">
@@ -19451,7 +19450,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="277" spans="1:18" hidden="1">
+    <row r="277" spans="1:18">
       <c r="A277" s="2"/>
       <c r="B277" s="2"/>
       <c r="C277" s="2" t="s">
@@ -19501,7 +19500,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="278" spans="1:18" hidden="1">
+    <row r="278" spans="1:18">
       <c r="A278" s="2"/>
       <c r="B278" s="2"/>
       <c r="C278" s="2" t="s">
@@ -19551,7 +19550,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="279" spans="1:18" hidden="1">
+    <row r="279" spans="1:18">
       <c r="A279" s="2"/>
       <c r="B279" s="2"/>
       <c r="C279" s="2" t="s">
@@ -19601,7 +19600,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="280" spans="1:18" hidden="1">
+    <row r="280" spans="1:18">
       <c r="A280" s="2"/>
       <c r="B280" s="2"/>
       <c r="C280" s="2" t="s">
@@ -19651,7 +19650,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="281" spans="1:18" hidden="1">
+    <row r="281" spans="1:18">
       <c r="A281" s="2"/>
       <c r="B281" s="2"/>
       <c r="C281" s="2" t="s">
@@ -19701,7 +19700,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="282" spans="1:18" hidden="1">
+    <row r="282" spans="1:18">
       <c r="A282" s="2"/>
       <c r="B282" s="2"/>
       <c r="C282" s="2" t="s">
@@ -19751,7 +19750,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="283" spans="1:18" hidden="1">
+    <row r="283" spans="1:18">
       <c r="A283" s="2"/>
       <c r="B283" s="2"/>
       <c r="C283" s="2" t="s">
@@ -19801,7 +19800,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="284" spans="1:18" hidden="1">
+    <row r="284" spans="1:18">
       <c r="A284" s="2"/>
       <c r="B284" s="2"/>
       <c r="C284" s="2" t="s">
@@ -19851,7 +19850,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="285" spans="1:18" hidden="1">
+    <row r="285" spans="1:18">
       <c r="A285" s="2"/>
       <c r="B285" s="2"/>
       <c r="C285" s="2" t="s">
@@ -19901,7 +19900,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="286" spans="1:18" hidden="1">
+    <row r="286" spans="1:18">
       <c r="A286" s="2"/>
       <c r="B286" s="2"/>
       <c r="C286" s="2" t="s">
@@ -19953,7 +19952,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="287" spans="1:18" hidden="1">
+    <row r="287" spans="1:18">
       <c r="A287" s="2"/>
       <c r="B287" s="2"/>
       <c r="C287" s="2" t="s">
@@ -20005,7 +20004,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="288" spans="1:18" hidden="1">
+    <row r="288" spans="1:18">
       <c r="A288" s="2"/>
       <c r="B288" s="2"/>
       <c r="C288" s="2" t="s">
@@ -20057,7 +20056,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="289" spans="1:18" hidden="1">
+    <row r="289" spans="1:18">
       <c r="A289" s="2"/>
       <c r="B289" s="2"/>
       <c r="C289" s="2" t="s">
@@ -20109,7 +20108,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="290" spans="1:18" hidden="1">
+    <row r="290" spans="1:18">
       <c r="A290" s="2"/>
       <c r="B290" s="2"/>
       <c r="C290" s="2" t="s">
@@ -20159,7 +20158,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="291" spans="1:18" hidden="1">
+    <row r="291" spans="1:18">
       <c r="A291" s="2"/>
       <c r="B291" s="2"/>
       <c r="C291" s="2" t="s">
@@ -20209,7 +20208,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="292" spans="1:18" hidden="1">
+    <row r="292" spans="1:18">
       <c r="A292" s="2"/>
       <c r="B292" s="2"/>
       <c r="C292" s="2" t="s">
@@ -20259,7 +20258,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="293" spans="1:18" hidden="1">
+    <row r="293" spans="1:18">
       <c r="A293" s="2"/>
       <c r="B293" s="2"/>
       <c r="C293" s="2" t="s">
@@ -20309,7 +20308,7 @@
         <v>1187</v>
       </c>
     </row>
-    <row r="294" spans="1:18" hidden="1">
+    <row r="294" spans="1:18">
       <c r="A294" s="2"/>
       <c r="B294" s="2"/>
       <c r="C294" s="2" t="s">
@@ -20359,7 +20358,7 @@
         <v>1187</v>
       </c>
     </row>
-    <row r="295" spans="1:18" hidden="1">
+    <row r="295" spans="1:18">
       <c r="A295" s="2"/>
       <c r="B295" s="2"/>
       <c r="C295" s="2" t="s">
@@ -20409,7 +20408,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="296" spans="1:18" hidden="1">
+    <row r="296" spans="1:18">
       <c r="A296" s="2"/>
       <c r="B296" s="2"/>
       <c r="C296" s="2" t="s">
@@ -20459,7 +20458,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="297" spans="1:18" hidden="1">
+    <row r="297" spans="1:18">
       <c r="A297" s="2"/>
       <c r="B297" s="2"/>
       <c r="C297" s="2" t="s">
@@ -20509,7 +20508,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="298" spans="1:18" hidden="1">
+    <row r="298" spans="1:18">
       <c r="A298" s="2"/>
       <c r="B298" s="2"/>
       <c r="C298" s="2" t="s">
@@ -20559,7 +20558,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="299" spans="1:18" hidden="1">
+    <row r="299" spans="1:18">
       <c r="A299" s="2"/>
       <c r="B299" s="2"/>
       <c r="C299" s="2" t="s">
@@ -20817,7 +20816,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="304" spans="1:18" hidden="1">
+    <row r="304" spans="1:18">
       <c r="A304" s="2"/>
       <c r="B304" s="2"/>
       <c r="C304" s="2" t="s">
@@ -20869,7 +20868,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="305" spans="1:18" hidden="1">
+    <row r="305" spans="1:18">
       <c r="A305" s="2"/>
       <c r="B305" s="2"/>
       <c r="C305" s="2" t="s">
@@ -21077,7 +21076,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="309" spans="1:18" hidden="1">
+    <row r="309" spans="1:18">
       <c r="A309" s="2"/>
       <c r="B309" s="2"/>
       <c r="C309" s="2" t="s">
@@ -21127,7 +21126,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="310" spans="1:18" hidden="1">
+    <row r="310" spans="1:18">
       <c r="A310" s="2"/>
       <c r="B310" s="2"/>
       <c r="C310" s="2" t="s">
@@ -21177,7 +21176,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="311" spans="1:18" hidden="1">
+    <row r="311" spans="1:18">
       <c r="A311" s="2"/>
       <c r="B311" s="2"/>
       <c r="C311" s="2" t="s">
@@ -21229,7 +21228,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="312" spans="1:18" hidden="1">
+    <row r="312" spans="1:18">
       <c r="A312" s="2"/>
       <c r="B312" s="2"/>
       <c r="C312" s="2" t="s">
@@ -21279,7 +21278,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="313" spans="1:18" hidden="1">
+    <row r="313" spans="1:18">
       <c r="A313" s="2"/>
       <c r="B313" s="2"/>
       <c r="C313" s="2" t="s">
@@ -21745,7 +21744,7 @@
         <v>1285</v>
       </c>
     </row>
-    <row r="322" spans="1:18" hidden="1">
+    <row r="322" spans="1:18">
       <c r="A322" s="2"/>
       <c r="B322" s="2"/>
       <c r="C322" s="2" t="s">
@@ -21849,7 +21848,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="324" spans="1:18" hidden="1">
+    <row r="324" spans="1:18">
       <c r="A324" s="2"/>
       <c r="B324" s="2"/>
       <c r="C324" s="2" t="s">
@@ -21899,7 +21898,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="325" spans="1:18" hidden="1">
+    <row r="325" spans="1:18">
       <c r="A325" s="2"/>
       <c r="B325" s="2"/>
       <c r="C325" s="2" t="s">
@@ -21949,7 +21948,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="326" spans="1:18" hidden="1">
+    <row r="326" spans="1:18">
       <c r="A326" s="2"/>
       <c r="B326" s="2"/>
       <c r="C326" s="2" t="s">
@@ -22103,7 +22102,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="329" spans="1:18" hidden="1">
+    <row r="329" spans="1:18">
       <c r="A329" s="2"/>
       <c r="B329" s="2"/>
       <c r="C329" s="2" t="s">
@@ -22153,7 +22152,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="330" spans="1:18" hidden="1">
+    <row r="330" spans="1:18">
       <c r="A330" s="2"/>
       <c r="B330" s="2"/>
       <c r="C330" s="2" t="s">
@@ -22463,7 +22462,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="336" spans="1:18" hidden="1">
+    <row r="336" spans="1:18">
       <c r="A336" s="2"/>
       <c r="B336" s="2"/>
       <c r="C336" s="2" t="s">
@@ -22515,7 +22514,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="337" spans="1:18" hidden="1">
+    <row r="337" spans="1:18">
       <c r="A337" s="2"/>
       <c r="B337" s="2"/>
       <c r="C337" s="2" t="s">
@@ -22567,7 +22566,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="338" spans="1:18" hidden="1">
+    <row r="338" spans="1:18">
       <c r="A338" s="2"/>
       <c r="B338" s="2"/>
       <c r="C338" s="2" t="s">
@@ -22617,7 +22616,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="339" spans="1:18" hidden="1">
+    <row r="339" spans="1:18">
       <c r="A339" s="2"/>
       <c r="B339" s="2"/>
       <c r="C339" s="2" t="s">
@@ -22667,7 +22666,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="340" spans="1:18" hidden="1">
+    <row r="340" spans="1:18">
       <c r="A340" s="2"/>
       <c r="B340" s="2"/>
       <c r="C340" s="2" t="s">
@@ -22719,7 +22718,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="341" spans="1:18" hidden="1">
+    <row r="341" spans="1:18">
       <c r="A341" s="2"/>
       <c r="B341" s="2"/>
       <c r="C341" s="2" t="s">
@@ -22771,7 +22770,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="342" spans="1:18" hidden="1">
+    <row r="342" spans="1:18">
       <c r="A342" s="2"/>
       <c r="B342" s="2"/>
       <c r="C342" s="2" t="s">
@@ -22821,7 +22820,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="343" spans="1:18" hidden="1">
+    <row r="343" spans="1:18">
       <c r="A343" s="2"/>
       <c r="B343" s="2"/>
       <c r="C343" s="2" t="s">
@@ -22923,7 +22922,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="345" spans="1:18" hidden="1">
+    <row r="345" spans="1:18">
       <c r="A345" s="2"/>
       <c r="B345" s="2"/>
       <c r="C345" s="2" t="s">
@@ -22973,7 +22972,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="346" spans="1:18" hidden="1">
+    <row r="346" spans="1:18">
       <c r="A346" s="2"/>
       <c r="B346" s="2"/>
       <c r="C346" s="2" t="s">
@@ -23023,7 +23022,7 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="347" spans="1:18" hidden="1">
+    <row r="347" spans="1:18">
       <c r="A347" s="2"/>
       <c r="B347" s="2"/>
       <c r="C347" s="2" t="s">
@@ -23073,7 +23072,7 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="348" spans="1:18" hidden="1">
+    <row r="348" spans="1:18">
       <c r="A348" s="2"/>
       <c r="B348" s="2"/>
       <c r="C348" s="2" t="s">
@@ -23123,7 +23122,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="349" spans="1:18" hidden="1">
+    <row r="349" spans="1:18">
       <c r="A349" s="2"/>
       <c r="B349" s="2"/>
       <c r="C349" s="2" t="s">
@@ -23175,7 +23174,7 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="350" spans="1:18" hidden="1">
+    <row r="350" spans="1:18">
       <c r="A350" s="2"/>
       <c r="B350" s="2"/>
       <c r="C350" s="2" t="s">
@@ -23227,7 +23226,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="351" spans="1:18" hidden="1">
+    <row r="351" spans="1:18">
       <c r="A351" s="2"/>
       <c r="B351" s="2"/>
       <c r="C351" s="2" t="s">
@@ -23279,7 +23278,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="352" spans="1:18" hidden="1">
+    <row r="352" spans="1:18">
       <c r="A352" s="2"/>
       <c r="B352" s="2"/>
       <c r="C352" s="2" t="s">
@@ -23383,7 +23382,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="354" spans="1:18" hidden="1">
+    <row r="354" spans="1:18">
       <c r="A354" s="2"/>
       <c r="B354" s="2"/>
       <c r="C354" s="2" t="s">
@@ -23433,7 +23432,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="355" spans="1:18" hidden="1">
+    <row r="355" spans="1:18">
       <c r="A355" s="2"/>
       <c r="B355" s="2"/>
       <c r="C355" s="2" t="s">
@@ -23483,7 +23482,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="356" spans="1:18" hidden="1">
+    <row r="356" spans="1:18">
       <c r="A356" s="2"/>
       <c r="B356" s="2"/>
       <c r="C356" s="2" t="s">
@@ -23637,7 +23636,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="359" spans="1:18" hidden="1">
+    <row r="359" spans="1:18">
       <c r="A359" s="2"/>
       <c r="B359" s="2"/>
       <c r="C359" s="2" t="s">
@@ -23689,7 +23688,7 @@
         <v>1433</v>
       </c>
     </row>
-    <row r="360" spans="1:18" hidden="1">
+    <row r="360" spans="1:18">
       <c r="A360" s="2"/>
       <c r="B360" s="2"/>
       <c r="C360" s="2" t="s">
@@ -23741,7 +23740,7 @@
         <v>1433</v>
       </c>
     </row>
-    <row r="361" spans="1:18" hidden="1">
+    <row r="361" spans="1:18">
       <c r="A361" s="2"/>
       <c r="B361" s="2"/>
       <c r="C361" s="2" t="s">
@@ -23791,7 +23790,7 @@
         <v>1438</v>
       </c>
     </row>
-    <row r="362" spans="1:18" hidden="1">
+    <row r="362" spans="1:18">
       <c r="A362" s="2"/>
       <c r="B362" s="2"/>
       <c r="C362" s="2" t="s">
@@ -23945,7 +23944,7 @@
         <v>1448</v>
       </c>
     </row>
-    <row r="365" spans="1:18" hidden="1">
+    <row r="365" spans="1:18">
       <c r="A365" s="2"/>
       <c r="B365" s="2"/>
       <c r="C365" s="2" t="s">
@@ -23997,7 +23996,7 @@
         <v>1453</v>
       </c>
     </row>
-    <row r="366" spans="1:18" hidden="1">
+    <row r="366" spans="1:18">
       <c r="A366" s="2"/>
       <c r="B366" s="2"/>
       <c r="C366" s="2" t="s">
@@ -24047,7 +24046,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="367" spans="1:18" hidden="1">
+    <row r="367" spans="1:18">
       <c r="A367" s="2"/>
       <c r="B367" s="2"/>
       <c r="C367" s="2" t="s">
@@ -24097,7 +24096,7 @@
         <v>1465</v>
       </c>
     </row>
-    <row r="368" spans="1:18" hidden="1">
+    <row r="368" spans="1:18">
       <c r="A368" s="2"/>
       <c r="B368" s="2"/>
       <c r="C368" s="2" t="s">
@@ -24407,7 +24406,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="374" spans="1:18" hidden="1">
+    <row r="374" spans="1:18">
       <c r="A374" s="2"/>
       <c r="B374" s="2"/>
       <c r="C374" s="2" t="s">
@@ -24457,7 +24456,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="375" spans="1:18" hidden="1">
+    <row r="375" spans="1:18">
       <c r="A375" s="2"/>
       <c r="B375" s="2"/>
       <c r="C375" s="2" t="s">
@@ -24507,7 +24506,7 @@
         <v>1497</v>
       </c>
     </row>
-    <row r="376" spans="1:18" hidden="1">
+    <row r="376" spans="1:18">
       <c r="A376" s="2"/>
       <c r="B376" s="2"/>
       <c r="C376" s="2" t="s">
@@ -24557,7 +24556,7 @@
         <v>1503</v>
       </c>
     </row>
-    <row r="377" spans="1:18" hidden="1">
+    <row r="377" spans="1:18">
       <c r="A377" s="2"/>
       <c r="B377" s="2"/>
       <c r="C377" s="2" t="s">
@@ -25179,7 +25178,7 @@
         <v>1539</v>
       </c>
     </row>
-    <row r="389" spans="1:18" hidden="1">
+    <row r="389" spans="1:18">
       <c r="A389" s="2"/>
       <c r="B389" s="2"/>
       <c r="C389" s="2" t="s">
@@ -25229,7 +25228,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="390" spans="1:18" hidden="1">
+    <row r="390" spans="1:18">
       <c r="A390" s="2"/>
       <c r="B390" s="2"/>
       <c r="C390" s="2" t="s">
@@ -25279,7 +25278,7 @@
         <v>1564</v>
       </c>
     </row>
-    <row r="391" spans="1:18" hidden="1">
+    <row r="391" spans="1:18">
       <c r="A391" s="2"/>
       <c r="B391" s="2"/>
       <c r="C391" s="2" t="s">
@@ -25329,7 +25328,7 @@
         <v>1564</v>
       </c>
     </row>
-    <row r="392" spans="1:18" hidden="1">
+    <row r="392" spans="1:18">
       <c r="A392" s="2"/>
       <c r="B392" s="2"/>
       <c r="C392" s="2" t="s">
@@ -25379,7 +25378,7 @@
         <v>1564</v>
       </c>
     </row>
-    <row r="393" spans="1:18" hidden="1">
+    <row r="393" spans="1:18">
       <c r="A393" s="2"/>
       <c r="B393" s="2"/>
       <c r="C393" s="2" t="s">
@@ -25429,7 +25428,7 @@
         <v>1564</v>
       </c>
     </row>
-    <row r="394" spans="1:18" hidden="1">
+    <row r="394" spans="1:18">
       <c r="A394" s="2"/>
       <c r="B394" s="2"/>
       <c r="C394" s="2" t="s">
@@ -25479,7 +25478,7 @@
         <v>1564</v>
       </c>
     </row>
-    <row r="395" spans="1:18" hidden="1">
+    <row r="395" spans="1:18">
       <c r="A395" s="2"/>
       <c r="B395" s="2"/>
       <c r="C395" s="2" t="s">
@@ -25529,7 +25528,7 @@
         <v>1564</v>
       </c>
     </row>
-    <row r="396" spans="1:18" hidden="1">
+    <row r="396" spans="1:18">
       <c r="A396" s="2"/>
       <c r="B396" s="2"/>
       <c r="C396" s="2" t="s">
@@ -25735,7 +25734,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="400" spans="1:18" hidden="1">
+    <row r="400" spans="1:18">
       <c r="A400" s="2"/>
       <c r="B400" s="2"/>
       <c r="C400" s="2" t="s">
@@ -25787,7 +25786,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="401" spans="1:18" hidden="1">
+    <row r="401" spans="1:18">
       <c r="A401" s="2"/>
       <c r="B401" s="2"/>
       <c r="C401" s="2" t="s">
@@ -25839,7 +25838,7 @@
         <v>1595</v>
       </c>
     </row>
-    <row r="402" spans="1:18" hidden="1">
+    <row r="402" spans="1:18">
       <c r="A402" s="2"/>
       <c r="B402" s="2"/>
       <c r="C402" s="2" t="s">
@@ -25891,7 +25890,7 @@
         <v>1595</v>
       </c>
     </row>
-    <row r="403" spans="1:18" hidden="1">
+    <row r="403" spans="1:18">
       <c r="A403" s="2"/>
       <c r="B403" s="2"/>
       <c r="C403" s="2" t="s">
@@ -25943,7 +25942,7 @@
         <v>1595</v>
       </c>
     </row>
-    <row r="404" spans="1:18" hidden="1">
+    <row r="404" spans="1:18">
       <c r="A404" s="2"/>
       <c r="B404" s="2"/>
       <c r="C404" s="2" t="s">
@@ -25995,7 +25994,7 @@
         <v>1595</v>
       </c>
     </row>
-    <row r="405" spans="1:18" hidden="1">
+    <row r="405" spans="1:18">
       <c r="A405" s="2"/>
       <c r="B405" s="2"/>
       <c r="C405" s="2" t="s">
@@ -26047,7 +26046,7 @@
         <v>1596</v>
       </c>
     </row>
-    <row r="406" spans="1:18" hidden="1">
+    <row r="406" spans="1:18">
       <c r="A406" s="2"/>
       <c r="B406" s="2"/>
       <c r="C406" s="2" t="s">
@@ -26099,7 +26098,7 @@
         <v>1596</v>
       </c>
     </row>
-    <row r="407" spans="1:18" hidden="1">
+    <row r="407" spans="1:18">
       <c r="A407" s="2"/>
       <c r="B407" s="2"/>
       <c r="C407" s="2" t="s">
@@ -26153,11 +26152,7 @@
     </row>
   </sheetData>
   <autoFilter ref="B1:R407">
-    <filterColumn colId="15">
-      <filters>
-        <filter val="Y"/>
-      </filters>
-    </filterColumn>
+    <filterColumn colId="15"/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding in "Called" column in call list
Adding in "Called" column in call list
</commit_message>
<xml_diff>
--- a/campaign/Advance Poll Kit/AdvancePoll.xlsx
+++ b/campaign/Advance Poll Kit/AdvancePoll.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2824" uniqueCount="772">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2825" uniqueCount="773">
   <si>
     <t>VotedOn</t>
   </si>
@@ -2333,6 +2333,9 @@
   </si>
   <si>
     <t>(905) 507-6540</t>
+  </si>
+  <si>
+    <t>Called</t>
   </si>
 </sst>
 </file>
@@ -2754,20 +2757,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L424"/>
+  <dimension ref="A1:M424"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2804,8 +2808,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="1" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="2"/>
       <c r="B2">
         <v>5</v>
@@ -2841,7 +2848,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" s="2"/>
       <c r="B3">
         <v>5</v>
@@ -2877,7 +2884,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" s="2"/>
       <c r="B4">
         <v>5</v>
@@ -2913,7 +2920,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" s="2"/>
       <c r="B5">
         <v>5</v>
@@ -2949,7 +2956,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6" s="2"/>
       <c r="B6">
         <v>5</v>
@@ -2985,7 +2992,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7" s="2"/>
       <c r="B7">
         <v>5</v>
@@ -3021,7 +3028,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13">
       <c r="A8" s="2"/>
       <c r="B8">
         <v>5</v>
@@ -3057,7 +3064,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:13">
       <c r="A9" s="2"/>
       <c r="B9">
         <v>5</v>
@@ -3090,7 +3097,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:13">
       <c r="A10" s="2"/>
       <c r="B10">
         <v>5</v>
@@ -3123,7 +3130,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:13">
       <c r="A11" s="2"/>
       <c r="B11">
         <v>5</v>
@@ -3156,7 +3163,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13">
       <c r="A12" s="2"/>
       <c r="B12">
         <v>5</v>
@@ -3192,7 +3199,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="A13" s="2"/>
       <c r="B13">
         <v>5</v>
@@ -3228,7 +3235,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:13">
       <c r="A14" s="2"/>
       <c r="B14">
         <v>5</v>
@@ -3264,7 +3271,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:13">
       <c r="A15" s="2"/>
       <c r="B15">
         <v>5</v>
@@ -3300,7 +3307,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:13">
       <c r="A16" s="2"/>
       <c r="B16">
         <v>5</v>

</xml_diff>